<commit_message>
print.xlsx 수정: 템플릿 업데이트 20250620
</commit_message>
<xml_diff>
--- a/print.xlsx
+++ b/print.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d30ae142562e1ddc/보험/한화라이프랩/자동화 프로그램 모음/bojang-v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{567D7A04-6FFF-4426-A8EA-D3603580CD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91B20E20-644F-43EE-84DE-18977EE6507D}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{567D7A04-6FFF-4426-A8EA-D3603580CD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A93962C3-4111-4948-A09A-735D5C66E3C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="기존 보험" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +456,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -870,7 +876,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1063,25 +1069,46 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="7" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1095,9 +1122,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1105,46 +1129,31 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1738,7 +1747,7 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="47.25" x14ac:dyDescent="0.3"/>
@@ -1752,9 +1761,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="274.5" customHeight="1" thickBot="1" x14ac:dyDescent="1.2">
-      <c r="A1" s="64"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
       <c r="D1" s="63"/>
       <c r="E1" s="63"/>
       <c r="F1" s="63"/>
@@ -1772,13 +1781,13 @@
       <c r="R1" s="63"/>
     </row>
     <row r="2" spans="1:18" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="84" t="s">
+      <c r="A2" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="81" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2"/>
@@ -1798,9 +1807,9 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="71"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="75"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1818,11 +1827,11 @@
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="93"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1840,11 +1849,11 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1862,11 +1871,11 @@
       <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -1884,14 +1893,14 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="86">
+      <c r="A7" s="64">
         <f t="shared" ref="A7:A48" si="0">SUM(D7:R7)</f>
         <v>0</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="83"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1909,86 +1918,86 @@
       <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="85">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B8" s="76" t="s">
+      <c r="A8" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B8" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="89"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="91"/>
     </row>
     <row r="9" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B9" s="79" t="s">
+      <c r="A9" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B9" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="90"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
     </row>
     <row r="10" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="87">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B10" s="79" t="s">
+      <c r="A10" s="89">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="91"/>
-      <c r="P10" s="91"/>
-      <c r="Q10" s="91"/>
-      <c r="R10" s="91"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="94"/>
+      <c r="O10" s="94"/>
+      <c r="P10" s="94"/>
+      <c r="Q10" s="94"/>
+      <c r="R10" s="94"/>
     </row>
     <row r="11" spans="1:18" ht="99.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="87" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -2015,7 +2024,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B12" s="68"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="11" t="s">
         <v>12</v>
       </c>
@@ -2040,7 +2049,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B13" s="68"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="14" t="s">
         <v>13</v>
       </c>
@@ -2065,7 +2074,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="65" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -2092,7 +2101,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B15" s="71"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="20" t="s">
         <v>16</v>
       </c>
@@ -2117,7 +2126,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="78" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -2144,7 +2153,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B17" s="68"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="26" t="s">
         <v>19</v>
       </c>
@@ -2169,7 +2178,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="65" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="29" t="s">
@@ -2196,7 +2205,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B19" s="68"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="32" t="s">
         <v>22</v>
       </c>
@@ -2221,7 +2230,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B20" s="71"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="35" t="s">
         <v>23</v>
       </c>
@@ -2246,7 +2255,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="65" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="38" t="s">
@@ -2273,7 +2282,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B22" s="71"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="41" t="s">
         <v>26</v>
       </c>
@@ -2298,7 +2307,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B23" s="78" t="s">
+      <c r="B23" s="69" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="17" t="s">
@@ -2325,7 +2334,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B24" s="68"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="44" t="s">
         <v>29</v>
       </c>
@@ -2350,7 +2359,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B25" s="68"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="44" t="s">
         <v>30</v>
       </c>
@@ -2375,7 +2384,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B26" s="68"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="44" t="s">
         <v>31</v>
       </c>
@@ -2400,7 +2409,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B27" s="68"/>
+      <c r="B27" s="66"/>
       <c r="C27" s="44" t="s">
         <v>32</v>
       </c>
@@ -2425,7 +2434,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B28" s="71"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="20" t="s">
         <v>33</v>
       </c>
@@ -2450,7 +2459,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="69" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="17" t="s">
@@ -2477,7 +2486,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B30" s="71"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="20" t="s">
         <v>36</v>
       </c>
@@ -2502,7 +2511,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B31" s="70" t="s">
+      <c r="B31" s="65" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="47" t="s">
@@ -2529,7 +2538,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B32" s="68"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="8" t="s">
         <v>39</v>
       </c>
@@ -2554,7 +2563,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B33" s="68"/>
+      <c r="B33" s="66"/>
       <c r="C33" s="11" t="s">
         <v>40</v>
       </c>
@@ -2579,7 +2588,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B34" s="71"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="20" t="s">
         <v>41</v>
       </c>
@@ -2604,7 +2613,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="69" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="49" t="s">
@@ -2631,7 +2640,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B36" s="68"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="50" t="s">
         <v>57</v>
       </c>
@@ -2656,7 +2665,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B37" s="68"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="50" t="s">
         <v>58</v>
       </c>
@@ -2681,7 +2690,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B38" s="68"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="50" t="s">
         <v>59</v>
       </c>
@@ -2706,7 +2715,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B39" s="68"/>
+      <c r="B39" s="66"/>
       <c r="C39" s="50" t="s">
         <v>60</v>
       </c>
@@ -2731,7 +2740,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B40" s="71"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="51" t="s">
         <v>61</v>
       </c>
@@ -2783,7 +2792,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B42" s="78" t="s">
+      <c r="B42" s="69" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="17" t="s">
@@ -2810,7 +2819,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B43" s="71"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="20" t="s">
         <v>47</v>
       </c>
@@ -2862,7 +2871,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B45" s="69" t="s">
+      <c r="B45" s="79" t="s">
         <v>50</v>
       </c>
       <c r="C45" s="17" t="s">
@@ -2889,7 +2898,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B46" s="68"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="44" t="s">
         <v>52</v>
       </c>
@@ -2914,7 +2923,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B47" s="68"/>
+      <c r="B47" s="66"/>
       <c r="C47" s="44" t="s">
         <v>53</v>
       </c>
@@ -2939,7 +2948,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B48" s="68"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="14" t="s">
         <v>54</v>
       </c>
@@ -3045,15 +3054,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B45:B48"/>
@@ -3067,6 +3067,15 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B35:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>